<commit_message>
added Subject to DataBase from ExcelFile
</commit_message>
<xml_diff>
--- a/docs/Subjects.xlsx
+++ b/docs/Subjects.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\KPandDP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CBA8CF-9646-4C21-B4B7-58A4716A17C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28551B9B-0420-4D8D-92FF-FD9193C71A75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022.12.02 Список ПОО" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2022.12.02 Список ПОО'!$A$1:$D$1433</definedName>
+  </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="3858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="3858">
   <si>
     <t>Администрация Советского района г. Гомеля</t>
   </si>
@@ -12114,8 +12117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1434" sqref="B1434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -22981,8 +22984,8 @@
       <c r="A776" s="6" t="s">
         <v>3410</v>
       </c>
-      <c r="B776" s="7" t="s">
-        <v>448</v>
+      <c r="B776" s="7">
+        <v>457896542</v>
       </c>
       <c r="C776" s="7" t="s">
         <v>1720</v>
@@ -27727,8 +27730,8 @@
       <c r="A1115" s="6" t="s">
         <v>3631</v>
       </c>
-      <c r="B1115" s="7" t="s">
-        <v>448</v>
+      <c r="B1115" s="7">
+        <v>123456879</v>
       </c>
       <c r="C1115" s="7" t="s">
         <v>2290</v>
@@ -32190,6 +32193,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1433" xr:uid="{4882638C-CB60-48E5-B8A7-EF1200208201}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Import Excel file to Data Base
</commit_message>
<xml_diff>
--- a/docs/Subjects.xlsx
+++ b/docs/Subjects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\KPandDP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1FD154-C62E-40E5-BC5C-C63737AE9D1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9FE3C7-7DAF-4C74-95F9-D285F999F1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12180,8 +12180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1425" workbookViewId="0">
+      <selection activeCell="A1442" sqref="A1442:XFD1442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>